<commit_message>
Saving treated datasets with new features
</commit_message>
<xml_diff>
--- a/Data/mercado-desafio-tratado.xlsx
+++ b/Data/mercado-desafio-tratado.xlsx
@@ -460,12 +460,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Variação</t>
+          <t>Change</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Variação Percentual</t>
+          <t>Percentage Change</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.7507638611178538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.7507638611178538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -703,10 +703,10 @@
         <v>4.991899967193604</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.452736915778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -723,10 +723,10 @@
         <v>4.991899967193604</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.452736915778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -843,10 +843,10 @@
         <v>4.972400188446045</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.08246163961050948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -863,10 +863,10 @@
         <v>4.972400188446045</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.08246163961050948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -983,10 +983,10 @@
         <v>4.962399959564209</v>
       </c>
       <c r="E27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5541704177811909</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1003,10 +1003,10 @@
         <v>4.962399959564209</v>
       </c>
       <c r="E28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5541704177811909</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1123,10 +1123,10 @@
         <v>4.969799995422363</v>
       </c>
       <c r="E34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0503049865741431</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1143,10 +1143,10 @@
         <v>4.969799995422363</v>
       </c>
       <c r="E35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0503049865741431</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.1986289845035179</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1286,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.1986289845035179</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1403,10 +1403,10 @@
         <v>4.992700099945068</v>
       </c>
       <c r="E48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.4706865062450509</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1423,10 +1423,10 @@
         <v>4.992700099945068</v>
       </c>
       <c r="E49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.4706865062450509</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1543,10 +1543,10 @@
         <v>4.974500179290771</v>
       </c>
       <c r="E55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>0.1668570532452005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1563,10 +1563,10 @@
         <v>4.974500179290771</v>
       </c>
       <c r="E56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.1668570532452005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1683,10 +1683,10 @@
         <v>5.014100074768066</v>
       </c>
       <c r="E62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>0.4746593782601212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1803,10 +1803,10 @@
         <v>5.057400226593018</v>
       </c>
       <c r="E68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>0.3717376081413996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1823,10 +1823,10 @@
         <v>5.057400226593018</v>
       </c>
       <c r="E69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>0.3717376081413996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1943,10 +1943,10 @@
         <v>5.090400218963623</v>
       </c>
       <c r="E75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>0.4754132958538194</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1963,10 +1963,10 @@
         <v>5.090400218963623</v>
       </c>
       <c r="E76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>0.4754132958538194</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2083,10 +2083,10 @@
         <v>5.241700172424316</v>
       </c>
       <c r="E82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>0.1736070364158134</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2103,10 +2103,10 @@
         <v>5.241700172424316</v>
       </c>
       <c r="E83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>0.1736070364158134</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2223,10 +2223,10 @@
         <v>5.158599853515625</v>
       </c>
       <c r="E89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>0.2539384868401592</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -2243,10 +2243,10 @@
         <v>5.158599853515625</v>
       </c>
       <c r="E90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>0.2539384868401592</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>-1.64569141806963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2386,7 +2386,7 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>-1.64569141806963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2503,10 +2503,10 @@
         <v>5.140799999237061</v>
       </c>
       <c r="E103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>1.029019559246562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -2523,10 +2523,10 @@
         <v>5.140799999237061</v>
       </c>
       <c r="E104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>1.029019559246562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -2646,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>-0.09749472221256304</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>-0.09749472221256304</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>-0.1555554855050065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -2806,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="F118" t="n">
-        <v>-0.1555554855050065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -3066,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="F131" t="n">
-        <v>-0.8236418200265615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>-0.8236418200265615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -3206,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>-0.7348571560704334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -3226,7 +3226,7 @@
         <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>-0.7348571560704334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -3343,10 +3343,10 @@
         <v>5.452400207519531</v>
       </c>
       <c r="E145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F145" t="n">
-        <v>0.5502202455163806</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -3363,10 +3363,10 @@
         <v>5.452400207519531</v>
       </c>
       <c r="E146" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>0.5502202455163806</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>-0.3999606428394025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -3506,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>-0.3999606428394025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -3626,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>-1.257651022548164</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -3646,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="F160" t="n">
-        <v>-1.257651022548164</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -3763,10 +3763,10 @@
         <v>5.438000202178955</v>
       </c>
       <c r="E166" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>0.4284694746627877</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -3783,10 +3783,10 @@
         <v>5.438000202178955</v>
       </c>
       <c r="E167" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F167" t="n">
-        <v>0.4284694746627877</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -3903,10 +3903,10 @@
         <v>5.543200016021729</v>
       </c>
       <c r="E173" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F173" t="n">
-        <v>1.001227275890536</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -3923,10 +3923,10 @@
         <v>5.543200016021729</v>
       </c>
       <c r="E174" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>1.001227275890536</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -4046,7 +4046,7 @@
         <v>0</v>
       </c>
       <c r="F180" t="n">
-        <v>-0.1860755871972966</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181">
@@ -4066,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="F181" t="n">
-        <v>-0.1860755871972966</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -4183,10 +4183,10 @@
         <v>5.75059986114502</v>
       </c>
       <c r="E187" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>1.634609691869291</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -4203,10 +4203,10 @@
         <v>5.75059986114502</v>
       </c>
       <c r="E188" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F188" t="n">
-        <v>1.634609691869291</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -4326,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>-1.617348099026611</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -4346,7 +4346,7 @@
         <v>0</v>
       </c>
       <c r="F195" t="n">
-        <v>-1.617348099026611</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -4463,10 +4463,10 @@
         <v>5.484899997711182</v>
       </c>
       <c r="E201" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F201" t="n">
-        <v>0.2917062118365746</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -4483,10 +4483,10 @@
         <v>5.484899997711182</v>
       </c>
       <c r="E202" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F202" t="n">
-        <v>0.2917062118365746</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -4603,10 +4603,10 @@
         <v>5.59089994430542</v>
       </c>
       <c r="E208" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F208" t="n">
-        <v>1.938862599783863</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -4623,10 +4623,10 @@
         <v>5.59089994430542</v>
       </c>
       <c r="E209" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F209" t="n">
-        <v>1.938862599783863</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -4743,10 +4743,10 @@
         <v>5.627699851989746</v>
       </c>
       <c r="E215" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F215" t="n">
-        <v>1.163881946175533</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216">
@@ -4763,10 +4763,10 @@
         <v>5.627699851989746</v>
       </c>
       <c r="E216" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F216" t="n">
-        <v>1.163881946175533</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -4886,7 +4886,7 @@
         <v>0</v>
       </c>
       <c r="F222" t="n">
-        <v>-1.338124515347604</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -4906,7 +4906,7 @@
         <v>0</v>
       </c>
       <c r="F223" t="n">
-        <v>-1.338124515347604</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -5026,7 +5026,7 @@
         <v>0</v>
       </c>
       <c r="F229" t="n">
-        <v>-0.7412390697094106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230">
@@ -5046,7 +5046,7 @@
         <v>0</v>
       </c>
       <c r="F230" t="n">
-        <v>-0.7412390697094106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -5166,7 +5166,7 @@
         <v>0</v>
       </c>
       <c r="F236" t="n">
-        <v>-0.6840066628318547</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -5186,7 +5186,7 @@
         <v>0</v>
       </c>
       <c r="F237" t="n">
-        <v>-0.6840066628318547</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238">
@@ -5306,7 +5306,7 @@
         <v>0</v>
       </c>
       <c r="F243" t="n">
-        <v>-0.6824050618922666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244">
@@ -5326,7 +5326,7 @@
         <v>0</v>
       </c>
       <c r="F244" t="n">
-        <v>-0.6824050618922666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245">
@@ -5443,10 +5443,10 @@
         <v>5.47629976272583</v>
       </c>
       <c r="E250" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F250" t="n">
-        <v>0.6573740754275735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251">
@@ -5463,10 +5463,10 @@
         <v>5.47629976272583</v>
       </c>
       <c r="E251" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F251" t="n">
-        <v>0.6573740754275735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252">
@@ -5586,7 +5586,7 @@
         <v>0</v>
       </c>
       <c r="F257" t="n">
-        <v>-0.2579860209660735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -5606,7 +5606,7 @@
         <v>0</v>
       </c>
       <c r="F258" t="n">
-        <v>-0.2579860209660735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259">
@@ -5726,7 +5726,7 @@
         <v>0</v>
       </c>
       <c r="F264" t="n">
-        <v>-0.286635499604984</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -5746,7 +5746,7 @@
         <v>0</v>
       </c>
       <c r="F265" t="n">
-        <v>-0.286635499604984</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266">
@@ -5866,7 +5866,7 @@
         <v>0</v>
       </c>
       <c r="F271" t="n">
-        <v>-0.3972464338027704</v>
+        <v>0</v>
       </c>
     </row>
     <row r="272">
@@ -5886,7 +5886,7 @@
         <v>0</v>
       </c>
       <c r="F272" t="n">
-        <v>-0.3972464338027704</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -5906,7 +5906,7 @@
         <v>0</v>
       </c>
       <c r="F273" t="n">
-        <v>-0.3972464338027704</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274">
@@ -6023,10 +6023,10 @@
         <v>5.789400100708008</v>
       </c>
       <c r="E279" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F279" t="n">
-        <v>0.4680983476827595</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280">
@@ -6043,10 +6043,10 @@
         <v>5.789400100708008</v>
       </c>
       <c r="E280" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F280" t="n">
-        <v>0.4680983476827595</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281">

</xml_diff>